<commit_message>
creating digikey cart, but without pin connectors and jtag
</commit_message>
<xml_diff>
--- a/LV3.1/RecoveryBoard/RecoveryBoard-BOM.xlsx
+++ b/LV3.1/RecoveryBoard/RecoveryBoard-BOM.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="215">
   <si>
     <t>Qty</t>
   </si>
@@ -1536,8 +1536,8 @@
   <dimension ref="A1:J49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E27" sqref="E27"/>
+      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G49" sqref="G49:J49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2862,11 +2862,15 @@
       <c r="G43" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="H43" s="6"/>
+      <c r="H43" s="6" t="s">
+        <v>198</v>
+      </c>
       <c r="I43" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="J43" s="6"/>
+        <v>199</v>
+      </c>
+      <c r="J43" s="6" t="s">
+        <v>200</v>
+      </c>
     </row>
     <row r="44" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="6">
@@ -3042,11 +3046,15 @@
       <c r="G49" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="H49" s="6"/>
+      <c r="H49" s="6" t="s">
+        <v>198</v>
+      </c>
       <c r="I49" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="J49" s="6"/>
+        <v>199</v>
+      </c>
+      <c r="J49" s="6" t="s">
+        <v>200</v>
+      </c>
     </row>
   </sheetData>
   <sortState ref="A2:X48">

</xml_diff>

<commit_message>
finished bom without jtag and connectors
</commit_message>
<xml_diff>
--- a/LV3.1/RecoveryBoard/RecoveryBoard-BOM.xlsx
+++ b/LV3.1/RecoveryBoard/RecoveryBoard-BOM.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="222">
   <si>
     <t>Qty</t>
   </si>
@@ -165,12 +165,6 @@
     <t>R1, R4, R16</t>
   </si>
   <si>
-    <t>1276-4275-1-ND</t>
-  </si>
-  <si>
-    <t>RC1005F6653CS</t>
-  </si>
-  <si>
     <t>10u</t>
   </si>
   <si>
@@ -664,6 +658,33 @@
   </si>
   <si>
     <t>RC0603FR-0751R1L</t>
+  </si>
+  <si>
+    <t>REVISIONS</t>
+  </si>
+  <si>
+    <t>REV DESCRIPTION</t>
+  </si>
+  <si>
+    <t>311-2092-1-ND</t>
+  </si>
+  <si>
+    <t>RT0603DRE0726K4L</t>
+  </si>
+  <si>
+    <t>R-US_0805-C-NOSILK</t>
+  </si>
+  <si>
+    <t>RHM470KBUCT-ND</t>
+  </si>
+  <si>
+    <t>LTR10EZPJ474</t>
+  </si>
+  <si>
+    <t>311-1.0KGRCT-ND</t>
+  </si>
+  <si>
+    <t>RC0603JR-071KL</t>
   </si>
 </sst>
 </file>
@@ -806,7 +827,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="36">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1001,6 +1022,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1180,7 +1207,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1212,6 +1239,11 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1533,11 +1565,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J49"/>
+  <dimension ref="A1:J51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G49" sqref="G49:J49"/>
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1591,7 +1623,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>10</v>
@@ -1607,7 +1639,7 @@
         <v>12</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="I2" s="7" t="s">
         <v>14</v>
@@ -1705,13 +1737,13 @@
         <v>12</v>
       </c>
       <c r="H6" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="J6" s="6" t="s">
         <v>141</v>
-      </c>
-      <c r="I6" s="7" t="s">
-        <v>142</v>
-      </c>
-      <c r="J6" s="6" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -1719,7 +1751,7 @@
         <v>1</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>30</v>
@@ -1728,7 +1760,7 @@
         <v>31</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="F7" s="7" t="s">
         <v>33</v>
@@ -1737,13 +1769,13 @@
         <v>12</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="J7" s="6" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -1769,13 +1801,13 @@
         <v>12</v>
       </c>
       <c r="H8" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="I8" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="J8" s="6" t="s">
         <v>144</v>
-      </c>
-      <c r="I8" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="J8" s="6" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -1801,13 +1833,13 @@
         <v>12</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="I9" s="7" t="s">
         <v>43</v>
       </c>
       <c r="J9" s="6" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -1833,13 +1865,13 @@
         <v>12</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="I10" s="7" t="s">
         <v>43</v>
       </c>
       <c r="J10" s="6" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -1847,16 +1879,16 @@
         <v>1</v>
       </c>
       <c r="B11" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="D11" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="C11" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="D11" s="6" t="s">
+      <c r="E11" s="6" t="s">
         <v>52</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>54</v>
       </c>
       <c r="F11" s="7" t="s">
         <v>41</v>
@@ -1865,13 +1897,13 @@
         <v>12</v>
       </c>
       <c r="H11" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="I11" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="J11" s="6" t="s">
         <v>151</v>
-      </c>
-      <c r="I11" s="7" t="s">
-        <v>152</v>
-      </c>
-      <c r="J11" s="6" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -1879,7 +1911,7 @@
         <v>1</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>30</v>
@@ -1888,7 +1920,7 @@
         <v>31</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F12" s="7" t="s">
         <v>33</v>
@@ -1897,13 +1929,13 @@
         <v>12</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="I12" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="J12" s="6" t="s">
         <v>159</v>
-      </c>
-      <c r="J12" s="6" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -1911,7 +1943,7 @@
         <v>1</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C13" s="6" t="s">
         <v>39</v>
@@ -1920,7 +1952,7 @@
         <v>31</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F13" s="7" t="s">
         <v>41</v>
@@ -1929,13 +1961,13 @@
         <v>12</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="J13" s="6" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -1943,7 +1975,7 @@
         <v>1</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>30</v>
@@ -1952,7 +1984,7 @@
         <v>31</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F14" s="7" t="s">
         <v>33</v>
@@ -1961,13 +1993,13 @@
         <v>12</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="I14" s="7" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="J14" s="6" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -1975,16 +2007,16 @@
         <v>1</v>
       </c>
       <c r="B15" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="E15" s="6" t="s">
         <v>69</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>71</v>
       </c>
       <c r="F15" s="7" t="s">
         <v>41</v>
@@ -1993,13 +2025,13 @@
         <v>12</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="I15" s="7" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="J15" s="6" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -2007,16 +2039,16 @@
         <v>1</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F16" s="7" t="s">
         <v>41</v>
@@ -2025,13 +2057,13 @@
         <v>12</v>
       </c>
       <c r="H16" s="6" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="I16" s="7" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="J16" s="6" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -2039,7 +2071,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C17" s="6" t="s">
         <v>30</v>
@@ -2048,7 +2080,7 @@
         <v>31</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F17" s="7" t="s">
         <v>33</v>
@@ -2057,13 +2089,13 @@
         <v>12</v>
       </c>
       <c r="H17" s="6" t="s">
-        <v>48</v>
+        <v>215</v>
       </c>
       <c r="I17" s="7" t="s">
-        <v>43</v>
+        <v>197</v>
       </c>
       <c r="J17" s="6" t="s">
-        <v>49</v>
+        <v>216</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2071,7 +2103,7 @@
         <v>1</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C18" s="6" t="s">
         <v>30</v>
@@ -2080,7 +2112,7 @@
         <v>31</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F18" s="7" t="s">
         <v>33</v>
@@ -2089,13 +2121,13 @@
         <v>12</v>
       </c>
       <c r="H18" s="6" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="I18" s="7" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="J18" s="6" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
@@ -2103,7 +2135,7 @@
         <v>1</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C19" s="6" t="s">
         <v>15</v>
@@ -2112,7 +2144,7 @@
         <v>15</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F19" s="7"/>
       <c r="G19" s="6" t="s">
@@ -2128,21 +2160,21 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="6">
         <v>1</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>30</v>
+        <v>217</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>31</v>
+        <v>50</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F20" s="7" t="s">
         <v>33</v>
@@ -2151,13 +2183,13 @@
         <v>12</v>
       </c>
       <c r="H20" s="6" t="s">
-        <v>48</v>
+        <v>218</v>
       </c>
       <c r="I20" s="7" t="s">
-        <v>43</v>
+        <v>145</v>
       </c>
       <c r="J20" s="6" t="s">
-        <v>49</v>
+        <v>219</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2174,7 +2206,7 @@
         <v>31</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F21" s="7" t="s">
         <v>33</v>
@@ -2183,13 +2215,13 @@
         <v>12</v>
       </c>
       <c r="H21" s="6" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="I21" s="7" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="J21" s="6" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2197,31 +2229,31 @@
         <v>1</v>
       </c>
       <c r="B22" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="E22" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="C22" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="D22" s="6" t="s">
+      <c r="F22" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="E22" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="F22" s="7" t="s">
-        <v>88</v>
-      </c>
       <c r="G22" s="6" t="s">
         <v>12</v>
       </c>
       <c r="H22" s="6" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="I22" s="7" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="J22" s="6" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2229,31 +2261,31 @@
         <v>1</v>
       </c>
       <c r="B23" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="E23" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="C23" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="D23" s="6" t="s">
+      <c r="F23" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="E23" s="6" t="s">
+      <c r="G23" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H23" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="F23" s="7" t="s">
+      <c r="I23" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="G23" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="H23" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="I23" s="7" t="s">
-        <v>101</v>
-      </c>
       <c r="J23" s="6" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="24" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -2261,24 +2293,24 @@
         <v>1</v>
       </c>
       <c r="B24" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="E24" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="C24" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="D24" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="E24" s="8" t="s">
-        <v>104</v>
-      </c>
       <c r="F24" s="9" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="G24" s="8"/>
       <c r="H24" s="8"/>
       <c r="I24" s="9" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="J24" s="8"/>
     </row>
@@ -2287,31 +2319,31 @@
         <v>1</v>
       </c>
       <c r="B25" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="E25" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="C25" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="D25" s="6" t="s">
+      <c r="F25" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="E25" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="F25" s="7" t="s">
-        <v>110</v>
-      </c>
       <c r="G25" s="6" t="s">
         <v>12</v>
       </c>
       <c r="H25" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="I25" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="J25" s="6" t="s">
         <v>176</v>
-      </c>
-      <c r="I25" s="7" t="s">
-        <v>177</v>
-      </c>
-      <c r="J25" s="6" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -2319,31 +2351,31 @@
         <v>1</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="G26" s="6" t="s">
         <v>12</v>
       </c>
       <c r="H26" s="6" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="I26" s="7" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="J26" s="6" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -2351,31 +2383,31 @@
         <v>1</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F27" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="G27" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H27" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="I27" s="7" t="s">
         <v>182</v>
       </c>
-      <c r="G27" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="H27" s="6" t="s">
-        <v>181</v>
-      </c>
-      <c r="I27" s="7" t="s">
-        <v>184</v>
-      </c>
       <c r="J27" s="6" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
@@ -2383,31 +2415,31 @@
         <v>1</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G28" s="6" t="s">
         <v>12</v>
       </c>
       <c r="H28" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="I28" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="J28" s="6" t="s">
         <v>185</v>
-      </c>
-      <c r="I28" s="7" t="s">
-        <v>186</v>
-      </c>
-      <c r="J28" s="6" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2415,31 +2447,31 @@
         <v>1</v>
       </c>
       <c r="B29" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="D29" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="C29" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="D29" s="6" t="s">
+      <c r="E29" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="F29" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="E29" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="F29" s="7" t="s">
-        <v>122</v>
-      </c>
       <c r="G29" s="6" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="H29" s="6" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="I29" s="7" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="J29" s="6" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
@@ -2447,31 +2479,31 @@
         <v>1</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F30" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="G30" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H30" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="I30" s="7" t="s">
         <v>189</v>
       </c>
-      <c r="G30" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="H30" s="6" t="s">
-        <v>190</v>
-      </c>
-      <c r="I30" s="7" t="s">
-        <v>191</v>
-      </c>
       <c r="J30" s="6" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2479,31 +2511,31 @@
         <v>1</v>
       </c>
       <c r="B31" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="E31" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="C31" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="D31" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="E31" s="6" t="s">
-        <v>130</v>
-      </c>
       <c r="F31" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="G31" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H31" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="I31" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="J31" s="6" t="s">
         <v>192</v>
-      </c>
-      <c r="G31" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="H31" s="6" t="s">
-        <v>193</v>
-      </c>
-      <c r="I31" s="7" t="s">
-        <v>177</v>
-      </c>
-      <c r="J31" s="6" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -2511,31 +2543,31 @@
         <v>1</v>
       </c>
       <c r="B32" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="E32" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="C32" s="6" t="s">
+      <c r="F32" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="D32" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="E32" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="F32" s="7" t="s">
-        <v>137</v>
-      </c>
       <c r="G32" s="6" t="s">
         <v>12</v>
       </c>
       <c r="H32" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="I32" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="J32" s="6" t="s">
         <v>195</v>
-      </c>
-      <c r="I32" s="7" t="s">
-        <v>196</v>
-      </c>
-      <c r="J32" s="6" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="33" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -2565,16 +2597,16 @@
         <v>2</v>
       </c>
       <c r="B34" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="C34" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="D34" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="C34" s="14" t="s">
+      <c r="E34" s="14" t="s">
         <v>58</v>
-      </c>
-      <c r="D34" s="14" t="s">
-        <v>59</v>
-      </c>
-      <c r="E34" s="14" t="s">
-        <v>60</v>
       </c>
       <c r="F34" s="15">
         <v>304010013</v>
@@ -2583,13 +2615,13 @@
         <v>12</v>
       </c>
       <c r="H34" s="14" t="s">
+        <v>204</v>
+      </c>
+      <c r="I34" s="15" t="s">
         <v>206</v>
       </c>
-      <c r="I34" s="15" t="s">
-        <v>208</v>
-      </c>
       <c r="J34" s="14" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
@@ -2597,7 +2629,7 @@
         <v>2</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C35" s="6" t="s">
         <v>39</v>
@@ -2606,7 +2638,7 @@
         <v>31</v>
       </c>
       <c r="E35" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F35" s="7" t="s">
         <v>41</v>
@@ -2615,13 +2647,13 @@
         <v>12</v>
       </c>
       <c r="H35" s="6" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="I35" s="7" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="J35" s="6" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
@@ -2629,16 +2661,16 @@
         <v>2</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E36" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F36" s="7" t="s">
         <v>41</v>
@@ -2647,13 +2679,13 @@
         <v>12</v>
       </c>
       <c r="H36" s="6" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="I36" s="7" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="J36" s="6" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
@@ -2670,7 +2702,7 @@
         <v>31</v>
       </c>
       <c r="E37" s="6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F37" s="7" t="s">
         <v>33</v>
@@ -2679,13 +2711,13 @@
         <v>12</v>
       </c>
       <c r="H37" s="6" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="I37" s="7" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="J37" s="6" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
@@ -2702,7 +2734,7 @@
         <v>31</v>
       </c>
       <c r="E38" s="6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F38" s="7" t="s">
         <v>33</v>
@@ -2711,13 +2743,13 @@
         <v>12</v>
       </c>
       <c r="H38" s="6" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="I38" s="7" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="J38" s="6" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="39" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -2725,31 +2757,31 @@
         <v>2</v>
       </c>
       <c r="B39" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="D39" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="E39" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="F39" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="G39" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H39" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="C39" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="D39" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="E39" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="F39" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="G39" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="H39" s="6" t="s">
-        <v>91</v>
-      </c>
       <c r="I39" s="7" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="J39" s="6" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2757,31 +2789,31 @@
         <v>2</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E40" s="6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F40" s="7" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="G40" s="6" t="s">
         <v>12</v>
       </c>
       <c r="H40" s="6" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="I40" s="7" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="J40" s="6" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="41" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
@@ -2789,7 +2821,7 @@
         <v>1</v>
       </c>
       <c r="B41" s="11" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C41" s="11" t="s">
         <v>30</v>
@@ -2798,7 +2830,7 @@
         <v>31</v>
       </c>
       <c r="E41" s="11" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F41" s="12" t="s">
         <v>33</v>
@@ -2813,31 +2845,31 @@
         <v>2</v>
       </c>
       <c r="B42" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="C42" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="D42" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="C42" s="6" t="s">
+      <c r="E42" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="D42" s="6" t="s">
+      <c r="F42" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="E42" s="6" t="s">
+      <c r="G42" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H42" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="F42" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="G42" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="H42" s="6" t="s">
-        <v>123</v>
-      </c>
       <c r="I42" s="7" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="J42" s="6" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
@@ -2863,13 +2895,13 @@
         <v>12</v>
       </c>
       <c r="H43" s="6" t="s">
+        <v>196</v>
+      </c>
+      <c r="I43" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="J43" s="6" t="s">
         <v>198</v>
-      </c>
-      <c r="I43" s="7" t="s">
-        <v>199</v>
-      </c>
-      <c r="J43" s="6" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2877,31 +2909,31 @@
         <v>3</v>
       </c>
       <c r="B44" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="C44" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="D44" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="E44" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="C44" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="D44" s="6" t="s">
+      <c r="F44" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="E44" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="F44" s="7" t="s">
-        <v>95</v>
-      </c>
       <c r="G44" s="6" t="s">
         <v>12</v>
       </c>
       <c r="H44" s="6" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I44" s="7" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="J44" s="6" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
@@ -2909,16 +2941,16 @@
         <v>5</v>
       </c>
       <c r="B45" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C45" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="D45" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="C45" s="6" t="s">
+      <c r="E45" s="6" t="s">
         <v>51</v>
-      </c>
-      <c r="D45" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="E45" s="6" t="s">
-        <v>53</v>
       </c>
       <c r="F45" s="7" t="s">
         <v>41</v>
@@ -2927,13 +2959,13 @@
         <v>12</v>
       </c>
       <c r="H45" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="I45" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="J45" s="6" t="s">
         <v>151</v>
-      </c>
-      <c r="I45" s="7" t="s">
-        <v>152</v>
-      </c>
-      <c r="J45" s="6" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
@@ -2959,13 +2991,13 @@
         <v>12</v>
       </c>
       <c r="H46" s="6" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="I46" s="7" t="s">
         <v>43</v>
       </c>
       <c r="J46" s="6" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
@@ -2973,7 +3005,7 @@
         <v>7</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C47" s="6" t="s">
         <v>30</v>
@@ -2982,7 +3014,7 @@
         <v>31</v>
       </c>
       <c r="E47" s="6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F47" s="7" t="s">
         <v>33</v>
@@ -2991,13 +3023,13 @@
         <v>12</v>
       </c>
       <c r="H47" s="6" t="s">
-        <v>198</v>
+        <v>220</v>
       </c>
       <c r="I47" s="7" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="J47" s="6" t="s">
-        <v>200</v>
+        <v>221</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
@@ -3005,19 +3037,19 @@
         <v>9</v>
       </c>
       <c r="B48" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="C48" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="D48" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="E48" s="6" t="s">
         <v>131</v>
       </c>
-      <c r="C48" s="6" t="s">
-        <v>131</v>
-      </c>
-      <c r="D48" s="6" t="s">
-        <v>132</v>
-      </c>
-      <c r="E48" s="6" t="s">
-        <v>133</v>
-      </c>
       <c r="F48" s="7" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="G48" s="6"/>
       <c r="H48" s="6"/>
@@ -3047,14 +3079,24 @@
         <v>12</v>
       </c>
       <c r="H49" s="6" t="s">
+        <v>196</v>
+      </c>
+      <c r="I49" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="J49" s="6" t="s">
         <v>198</v>
       </c>
-      <c r="I49" s="7" t="s">
-        <v>199</v>
-      </c>
-      <c r="J49" s="6" t="s">
-        <v>200</v>
-      </c>
+    </row>
+    <row r="51" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B51" s="17" t="s">
+        <v>213</v>
+      </c>
+      <c r="C51" s="17" t="s">
+        <v>214</v>
+      </c>
+      <c r="F51" s="19"/>
+      <c r="I51" s="19"/>
     </row>
   </sheetData>
   <sortState ref="A2:X48">

</xml_diff>

<commit_message>
found samtec connector for jtag; still need pin connectors
</commit_message>
<xml_diff>
--- a/LV3.1/RecoveryBoard/RecoveryBoard-BOM.xlsx
+++ b/LV3.1/RecoveryBoard/RecoveryBoard-BOM.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="224">
   <si>
     <t>Qty</t>
   </si>
@@ -537,9 +537,6 @@
     <t>ESR03EZPJ751</t>
   </si>
   <si>
-    <t>Samtec</t>
-  </si>
-  <si>
     <t>JTAG Connector</t>
   </si>
   <si>
@@ -685,6 +682,15 @@
   </si>
   <si>
     <t>RC0603JR-071KL</t>
+  </si>
+  <si>
+    <t>SAM13164CT-ND</t>
+  </si>
+  <si>
+    <t>Samtec Inc.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> FTSH-105-01-L-DV-K-P-TR</t>
   </si>
 </sst>
 </file>
@@ -1568,8 +1574,8 @@
   <dimension ref="A1:J51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E43" sqref="E43"/>
+      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1583,7 +1589,7 @@
     <col min="7" max="7" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="22.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.7109375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1751,7 +1757,7 @@
         <v>1</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>30</v>
@@ -1760,7 +1766,7 @@
         <v>31</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F7" s="7" t="s">
         <v>33</v>
@@ -1769,13 +1775,13 @@
         <v>12</v>
       </c>
       <c r="H7" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="J7" s="6" t="s">
         <v>202</v>
-      </c>
-      <c r="I7" s="7" t="s">
-        <v>197</v>
-      </c>
-      <c r="J7" s="6" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2089,13 +2095,13 @@
         <v>12</v>
       </c>
       <c r="H17" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="I17" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="J17" s="6" t="s">
         <v>215</v>
-      </c>
-      <c r="I17" s="7" t="s">
-        <v>197</v>
-      </c>
-      <c r="J17" s="6" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2168,7 +2174,7 @@
         <v>79</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D20" s="6" t="s">
         <v>50</v>
@@ -2183,13 +2189,13 @@
         <v>12</v>
       </c>
       <c r="H20" s="6" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="I20" s="7" t="s">
         <v>145</v>
       </c>
       <c r="J20" s="6" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2305,14 +2311,20 @@
         <v>102</v>
       </c>
       <c r="F24" s="9" t="s">
-        <v>173</v>
-      </c>
-      <c r="G24" s="8"/>
-      <c r="H24" s="8"/>
+        <v>172</v>
+      </c>
+      <c r="G24" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="H24" s="8" t="s">
+        <v>221</v>
+      </c>
       <c r="I24" s="9" t="s">
-        <v>172</v>
-      </c>
-      <c r="J24" s="8"/>
+        <v>222</v>
+      </c>
+      <c r="J24" s="8" t="s">
+        <v>223</v>
+      </c>
     </row>
     <row r="25" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="6">
@@ -2337,13 +2349,13 @@
         <v>12</v>
       </c>
       <c r="H25" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="I25" s="7" t="s">
         <v>174</v>
       </c>
-      <c r="I25" s="7" t="s">
+      <c r="J25" s="6" t="s">
         <v>175</v>
-      </c>
-      <c r="J25" s="6" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -2363,16 +2375,16 @@
         <v>110</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G26" s="6" t="s">
         <v>12</v>
       </c>
       <c r="H26" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="I26" s="7" t="s">
         <v>177</v>
-      </c>
-      <c r="I26" s="7" t="s">
-        <v>178</v>
       </c>
       <c r="J26" s="6" t="s">
         <v>109</v>
@@ -2395,16 +2407,16 @@
         <v>112</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G27" s="6" t="s">
         <v>12</v>
       </c>
       <c r="H27" s="6" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I27" s="7" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="J27" s="6" t="s">
         <v>111</v>
@@ -2427,19 +2439,19 @@
         <v>115</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G28" s="6" t="s">
         <v>12</v>
       </c>
       <c r="H28" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="I28" s="7" t="s">
         <v>183</v>
       </c>
-      <c r="I28" s="7" t="s">
+      <c r="J28" s="6" t="s">
         <v>184</v>
-      </c>
-      <c r="J28" s="6" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2491,16 +2503,16 @@
         <v>125</v>
       </c>
       <c r="F30" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="G30" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H30" s="6" t="s">
         <v>187</v>
       </c>
-      <c r="G30" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="H30" s="6" t="s">
+      <c r="I30" s="7" t="s">
         <v>188</v>
-      </c>
-      <c r="I30" s="7" t="s">
-        <v>189</v>
       </c>
       <c r="J30" s="6" t="s">
         <v>124</v>
@@ -2523,19 +2535,19 @@
         <v>128</v>
       </c>
       <c r="F31" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="G31" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H31" s="6" t="s">
         <v>190</v>
       </c>
-      <c r="G31" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="H31" s="6" t="s">
+      <c r="I31" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="J31" s="6" t="s">
         <v>191</v>
-      </c>
-      <c r="I31" s="7" t="s">
-        <v>175</v>
-      </c>
-      <c r="J31" s="6" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -2561,13 +2573,13 @@
         <v>12</v>
       </c>
       <c r="H32" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="I32" s="7" t="s">
         <v>193</v>
       </c>
-      <c r="I32" s="7" t="s">
+      <c r="J32" s="6" t="s">
         <v>194</v>
-      </c>
-      <c r="J32" s="6" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="33" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -2615,13 +2627,13 @@
         <v>12</v>
       </c>
       <c r="H34" s="14" t="s">
+        <v>203</v>
+      </c>
+      <c r="I34" s="15" t="s">
+        <v>205</v>
+      </c>
+      <c r="J34" s="14" t="s">
         <v>204</v>
-      </c>
-      <c r="I34" s="15" t="s">
-        <v>206</v>
-      </c>
-      <c r="J34" s="14" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
@@ -2647,13 +2659,13 @@
         <v>12</v>
       </c>
       <c r="H35" s="6" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="I35" s="7" t="s">
         <v>150</v>
       </c>
       <c r="J35" s="6" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
@@ -2711,13 +2723,13 @@
         <v>12</v>
       </c>
       <c r="H37" s="6" t="s">
+        <v>208</v>
+      </c>
+      <c r="I37" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="J37" s="6" t="s">
         <v>209</v>
-      </c>
-      <c r="I37" s="7" t="s">
-        <v>197</v>
-      </c>
-      <c r="J37" s="6" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
@@ -2743,13 +2755,13 @@
         <v>12</v>
       </c>
       <c r="H38" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="I38" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="J38" s="6" t="s">
         <v>211</v>
-      </c>
-      <c r="I38" s="7" t="s">
-        <v>197</v>
-      </c>
-      <c r="J38" s="6" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="39" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -2830,7 +2842,7 @@
         <v>31</v>
       </c>
       <c r="E41" s="11" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F41" s="12" t="s">
         <v>33</v>
@@ -2895,13 +2907,13 @@
         <v>12</v>
       </c>
       <c r="H43" s="6" t="s">
+        <v>195</v>
+      </c>
+      <c r="I43" s="7" t="s">
         <v>196</v>
       </c>
-      <c r="I43" s="7" t="s">
+      <c r="J43" s="6" t="s">
         <v>197</v>
-      </c>
-      <c r="J43" s="6" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3023,13 +3035,13 @@
         <v>12</v>
       </c>
       <c r="H47" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="I47" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="J47" s="6" t="s">
         <v>220</v>
-      </c>
-      <c r="I47" s="7" t="s">
-        <v>197</v>
-      </c>
-      <c r="J47" s="6" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
@@ -3079,21 +3091,21 @@
         <v>12</v>
       </c>
       <c r="H49" s="6" t="s">
+        <v>195</v>
+      </c>
+      <c r="I49" s="7" t="s">
         <v>196</v>
       </c>
-      <c r="I49" s="7" t="s">
+      <c r="J49" s="6" t="s">
         <v>197</v>
-      </c>
-      <c r="J49" s="6" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="51" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B51" s="17" t="s">
+        <v>212</v>
+      </c>
+      <c r="C51" s="17" t="s">
         <v>213</v>
-      </c>
-      <c r="C51" s="17" t="s">
-        <v>214</v>
       </c>
       <c r="F51" s="19"/>
       <c r="I51" s="19"/>

</xml_diff>